<commit_message>
Add JSON support for fraud detection report
</commit_message>
<xml_diff>
--- a/fraud_report_with_metadata_and_categories.xlsx
+++ b/fraud_report_with_metadata_and_categories.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,139 +626,76 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Spirometry (procedure)</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>15000</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>7786.47</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>7213.53</v>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Standard pregnancy test</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>5700</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>5656.6</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Legitimate</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>Prostatectomy</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="n">
+        <v>10500</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>6142.64</v>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>4357.36</v>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
         <is>
           <t>Fraud</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Standard pregnancy test</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>5700</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>5656.6</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>43.4</v>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>seasonique 91 day pack</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>431.4</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>Legitimate</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Throat culture (procedure)</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>2300</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>2020.43</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>279.57</v>
-      </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>Risk</t>
-        </is>
-      </c>
-    </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Upper arm X-ray</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>431.4</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1068.6</v>
-      </c>
-      <c r="E16" s="1" t="inlineStr">
-        <is>
-          <t>Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>Prostatectomy</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>10500</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>6142.64</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>4357.36</v>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>Fraud</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Intubation</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>440.38</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>59.62</v>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>Legitimate</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Total Invoice Amount</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>66433.10000000001</v>
+      <c r="B16" t="n">
+        <v>47633.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of browser_test.html For POST test
</commit_message>
<xml_diff>
--- a/fraud_report_with_metadata_and_categories.xlsx
+++ b/fraud_report_with_metadata_and_categories.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12345-ABP-001</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -626,76 +626,154 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>Spirometry (procedure)</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>7786.47</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>7213.53</v>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Standard pregnancy test</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B14" s="2" t="n">
         <v>5700</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C14" s="2" t="n">
         <v>5656.6</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D14" s="2" t="n">
         <v>43.4</v>
       </c>
-      <c r="E13" s="2" t="inlineStr">
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>Legitimate</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Throat culture (procedure)</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2300</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>2020.43</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>279.57</v>
+      </c>
+      <c r="E15" s="1" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Upper arm X-ray</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>431.4</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1068.6</v>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="inlineStr">
         <is>
           <t>Prostatectomy</t>
         </is>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B17" s="3" t="n">
         <v>10500</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C17" s="3" t="n">
         <v>6142.64</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D17" s="3" t="n">
         <v>4357.36</v>
       </c>
-      <c r="E14" s="3" t="inlineStr">
+      <c r="E17" s="3" t="inlineStr">
         <is>
           <t>Fraud</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>seasonique 91 day pack</t>
         </is>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B18" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C18" s="2" t="n">
         <v>431.4</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D18" s="2" t="n">
         <v>68.59999999999999</v>
       </c>
-      <c r="E15" s="2" t="inlineStr">
+      <c r="E18" s="2" t="inlineStr">
         <is>
           <t>Legitimate</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Total Invoice Amount</t>
         </is>
       </c>
-      <c r="B16" t="n">
-        <v>47633.1</v>
+      <c r="B19" t="n">
+        <v>66433.10000000001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="inlineStr">
+        <is>
+          <t>Overall Status</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="n"/>
+      <c r="C20" s="3" t="n"/>
+      <c r="D20" s="3" t="n"/>
+      <c r="E20" s="3" t="inlineStr">
+        <is>
+          <t>Fraud</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Addition of save-invoice-data API
</commit_message>
<xml_diff>
--- a/fraud_report_with_metadata_and_categories.xlsx
+++ b/fraud_report_with_metadata_and_categories.xlsx
@@ -26,7 +26,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -45,12 +45,6 @@
         <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -64,11 +58,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +455,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Absa Bank Bank Account</t>
+          <t>I&amp;M Bank Bank Account</t>
         </is>
       </c>
     </row>
@@ -474,7 +467,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0123 4567 8901</t>
+          <t>0754 8532 0632</t>
         </is>
       </c>
     </row>
@@ -486,7 +479,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Juma Joseph Invoice No</t>
+          <t>Tobi Brown policy Number</t>
         </is>
       </c>
     </row>
@@ -510,7 +503,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>WHJ7UI9O00PLQ</t>
+          <t>AHKJDGSH986K</t>
         </is>
       </c>
     </row>
@@ -544,17 +537,17 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Chlamydia antigen test</t>
+          <t>Digital examination of rectum</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>4433.1</v>
+        <v>800</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>2159.75</v>
+        <v>694.1799999999999</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2273.35</v>
+        <v>105.82</v>
       </c>
       <c r="E9" s="1" t="inlineStr">
         <is>
@@ -563,216 +556,108 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Allergy screening test</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Renal dialysis (procedure)</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>1750</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>928.42</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>821.58</v>
+      </c>
+      <c r="E10" s="1" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Urine screening test for</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>1906.61</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>93.39</v>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>Legitimate</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>cisplatin 50 mg injection</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>500</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <v>431.4</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>68.59999999999999</v>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>Legitimate</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>Intramuscular injection</t>
-        </is>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>5500</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>2544.08</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>2955.92</v>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="inlineStr">
-        <is>
-          <t>Colonoscopy</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="n">
-        <v>20500</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>11731.22</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>8768.780000000001</v>
-      </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>Fraud</t>
+      <c r="C12" t="n">
+        <v>1108.27</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-608.27</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Potential Underreporting</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>Spirometry (procedure)</t>
-        </is>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>15000</v>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>7786.47</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>7213.53</v>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>Fraud</t>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>albuterol 5 mg/ml inhalation</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>100</v>
+      </c>
+      <c r="C13" t="n">
+        <v>440.38</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-340.38</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Potential Underreporting</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Standard pregnancy test</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>5700</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>5656.6</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>43.4</v>
-      </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>Legitimate</t>
-        </is>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total Invoice Amount</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>5150</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>Throat culture (procedure)</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="n">
-        <v>2300</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>2020.43</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>279.57</v>
-      </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>Upper arm X-ray</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="n">
-        <v>1500</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>431.4</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1068.6</v>
-      </c>
-      <c r="E16" s="1" t="inlineStr">
-        <is>
-          <t>Risk</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="inlineStr">
-        <is>
-          <t>Prostatectomy</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>10500</v>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>6142.64</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>4357.36</v>
-      </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>Fraud</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>seasonique 91 day pack</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>431.4</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>68.59999999999999</v>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>Legitimate</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Total Invoice Amount</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>66433.10000000001</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Overall Status</t>
         </is>
       </c>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="3" t="n"/>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>Fraud</t>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Risky</t>
         </is>
       </c>
     </row>

</xml_diff>